<commit_message>
added a v2 for dutch grid
</commit_message>
<xml_diff>
--- a/NL_bus_input.xlsx
+++ b/NL_bus_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\304723\Documents\GitHub\CBC_RD_thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B933820E-3EA2-4EA9-B796-9AF18BCF0837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C896B6DF-DB16-4C3B-BAAC-39779A9FF0AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32100" yWindow="10515" windowWidth="19500" windowHeight="10485" activeTab="6" xr2:uid="{4D1B5A0D-1CEB-45D9-8796-95763D14CA6B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="5" xr2:uid="{4D1B5A0D-1CEB-45D9-8796-95763D14CA6B}"/>
   </bookViews>
   <sheets>
     <sheet name="title_page" sheetId="1" r:id="rId1"/>
@@ -533,7 +533,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2082,8 +2082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBB44F85-5F13-4E40-BB24-6694A7B82B38}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2122,7 +2122,7 @@
         <v>10</v>
       </c>
       <c r="D2">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E2" t="s">
         <v>18</v>
@@ -2148,7 +2148,7 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
         <v>18</v>
@@ -2175,8 +2175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50A915C1-4CB9-4DD7-B6E4-10F8FAF3EAA1}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2220,10 +2220,10 @@
         <v>7</v>
       </c>
       <c r="C2" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="3">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>18</v>
@@ -2232,7 +2232,7 @@
         <v>-10</v>
       </c>
       <c r="G2" s="3">
-        <v>200</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -2243,10 +2243,10 @@
         <v>8</v>
       </c>
       <c r="C3" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" s="3">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>18</v>
@@ -2266,10 +2266,10 @@
         <v>5</v>
       </c>
       <c r="C4" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="3">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>18</v>
@@ -2289,10 +2289,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" s="3">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>17</v>
@@ -2301,7 +2301,7 @@
         <v>500</v>
       </c>
       <c r="G5" s="3">
-        <v>500</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -2312,10 +2312,10 @@
         <v>4</v>
       </c>
       <c r="C6" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="3">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>18</v>
@@ -2335,10 +2335,10 @@
         <v>3</v>
       </c>
       <c r="C7" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" s="3">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>17</v>

</xml_diff>